<commit_message>
Alerts replaced with sweet alerts
</commit_message>
<xml_diff>
--- a/backend/media/invigilationFiles/Classroom.xlsx
+++ b/backend/media/invigilationFiles/Classroom.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D15"/>
+  <dimension ref="A1:D26"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -418,203 +418,357 @@
     </row>
     <row r="2">
       <c r="A2">
-        <v>5</v>
+        <v>28</v>
       </c>
       <c r="B2" t="str">
-        <v>RnD</v>
+        <v>Old Acad</v>
       </c>
       <c r="C2" t="str">
-        <v>C100</v>
+        <v>C01</v>
       </c>
       <c r="D2">
-        <v>100</v>
+        <v>106</v>
       </c>
     </row>
     <row r="3">
       <c r="A3">
-        <v>6</v>
+        <v>29</v>
       </c>
       <c r="B3" t="str">
-        <v>Library</v>
+        <v>Old Acad</v>
       </c>
       <c r="C3" t="str">
-        <v>C101</v>
+        <v>C02</v>
       </c>
       <c r="D3">
-        <v>100</v>
+        <v>42</v>
       </c>
     </row>
     <row r="4">
       <c r="A4">
-        <v>7</v>
+        <v>30</v>
       </c>
       <c r="B4" t="str">
-        <v>LHC</v>
+        <v>Old Acad</v>
       </c>
       <c r="C4" t="str">
-        <v>C111</v>
+        <v>C03</v>
       </c>
       <c r="D4">
-        <v>1000</v>
+        <v>18</v>
       </c>
     </row>
     <row r="5">
       <c r="A5">
-        <v>8</v>
+        <v>31</v>
       </c>
       <c r="B5" t="str">
-        <v>LHC</v>
+        <v>Old Acad</v>
       </c>
       <c r="C5" t="str">
-        <v>C1000</v>
+        <v>C11</v>
       </c>
       <c r="D5">
-        <v>1000</v>
+        <v>94</v>
       </c>
     </row>
     <row r="6">
       <c r="A6">
-        <v>9</v>
+        <v>32</v>
       </c>
       <c r="B6" t="str">
-        <v>RnD</v>
+        <v>Old Acad</v>
       </c>
       <c r="C6" t="str">
-        <v>C1001</v>
+        <v>C12</v>
       </c>
       <c r="D6">
-        <v>1001</v>
+        <v>39</v>
       </c>
     </row>
     <row r="7">
       <c r="A7">
-        <v>10</v>
+        <v>33</v>
       </c>
       <c r="B7" t="str">
-        <v>RnD</v>
+        <v>Old Acad</v>
       </c>
       <c r="C7" t="str">
-        <v>C1012</v>
+        <v>C13</v>
       </c>
       <c r="D7">
-        <v>1012</v>
+        <v>18</v>
       </c>
     </row>
     <row r="8">
       <c r="A8">
-        <v>19</v>
+        <v>34</v>
       </c>
       <c r="B8" t="str">
-        <v>LHC</v>
+        <v>Old Acad</v>
       </c>
       <c r="C8" t="str">
-        <v>C201</v>
+        <v>C21</v>
       </c>
       <c r="D8">
-        <v>100</v>
+        <v>80</v>
       </c>
     </row>
     <row r="9">
       <c r="A9">
-        <v>21</v>
+        <v>35</v>
       </c>
       <c r="B9" t="str">
-        <v>LHC</v>
+        <v>Old Acad</v>
       </c>
       <c r="C9" t="str">
-        <v>C01</v>
+        <v>C22</v>
       </c>
       <c r="D9">
-        <v>100</v>
+        <v>18</v>
       </c>
     </row>
     <row r="10">
       <c r="A10">
-        <v>22</v>
+        <v>36</v>
       </c>
       <c r="B10" t="str">
-        <v>LHC</v>
+        <v>Old Acad</v>
       </c>
       <c r="C10" t="str">
-        <v>C02</v>
+        <v>C24</v>
       </c>
       <c r="D10">
-        <v>100</v>
+        <v>18</v>
       </c>
     </row>
     <row r="11">
       <c r="A11">
-        <v>23</v>
+        <v>37</v>
       </c>
       <c r="B11" t="str">
         <v>LHC</v>
       </c>
       <c r="C11" t="str">
-        <v>C03</v>
+        <v>C101</v>
       </c>
       <c r="D11">
-        <v>100</v>
+        <v>169</v>
       </c>
     </row>
     <row r="12">
       <c r="A12">
-        <v>24</v>
+        <v>38</v>
       </c>
       <c r="B12" t="str">
         <v>LHC</v>
       </c>
       <c r="C12" t="str">
-        <v>C11</v>
+        <v>C102</v>
       </c>
       <c r="D12">
-        <v>100</v>
+        <v>281</v>
       </c>
     </row>
     <row r="13">
       <c r="A13">
-        <v>25</v>
+        <v>39</v>
       </c>
       <c r="B13" t="str">
         <v>LHC</v>
       </c>
       <c r="C13" t="str">
-        <v>C12</v>
+        <v>C201</v>
       </c>
       <c r="D13">
-        <v>100</v>
+        <v>177</v>
       </c>
     </row>
     <row r="14">
       <c r="A14">
-        <v>26</v>
+        <v>40</v>
       </c>
       <c r="B14" t="str">
         <v>LHC</v>
       </c>
       <c r="C14" t="str">
-        <v>C21</v>
+        <v>C208</v>
       </c>
       <c r="D14">
-        <v>100</v>
+        <v>20</v>
       </c>
     </row>
     <row r="15">
       <c r="A15">
-        <v>27</v>
+        <v>41</v>
       </c>
       <c r="B15" t="str">
         <v>LHC</v>
       </c>
       <c r="C15" t="str">
-        <v>C102</v>
+        <v>C209</v>
       </c>
       <c r="D15">
-        <v>100</v>
+        <v>22</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16">
+        <v>42</v>
+      </c>
+      <c r="B16" t="str">
+        <v>LHC</v>
+      </c>
+      <c r="C16" t="str">
+        <v>C210</v>
+      </c>
+      <c r="D16">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17">
+        <v>43</v>
+      </c>
+      <c r="B17" t="str">
+        <v>Old Acad</v>
+      </c>
+      <c r="C17" t="str">
+        <v>C211</v>
+      </c>
+      <c r="D17">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18">
+        <v>44</v>
+      </c>
+      <c r="B18" t="str">
+        <v>LHC</v>
+      </c>
+      <c r="C18" t="str">
+        <v>C212</v>
+      </c>
+      <c r="D18">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19">
+        <v>45</v>
+      </c>
+      <c r="B19" t="str">
+        <v>LHC</v>
+      </c>
+      <c r="C19" t="str">
+        <v>C213</v>
+      </c>
+      <c r="D19">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20">
+        <v>46</v>
+      </c>
+      <c r="B20" t="str">
+        <v>LHC</v>
+      </c>
+      <c r="C20" t="str">
+        <v>C214</v>
+      </c>
+      <c r="D20">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21">
+        <v>47</v>
+      </c>
+      <c r="B21" t="str">
+        <v>LHC</v>
+      </c>
+      <c r="C21" t="str">
+        <v>C215</v>
+      </c>
+      <c r="D21">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22">
+        <v>48</v>
+      </c>
+      <c r="B22" t="str">
+        <v>LHC</v>
+      </c>
+      <c r="C22" t="str">
+        <v>C216</v>
+      </c>
+      <c r="D22">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23">
+        <v>49</v>
+      </c>
+      <c r="B23" t="str">
+        <v>RnD</v>
+      </c>
+      <c r="C23" t="str">
+        <v>A006</v>
+      </c>
+      <c r="D23">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24">
+        <v>50</v>
+      </c>
+      <c r="B24" t="str">
+        <v>RnD</v>
+      </c>
+      <c r="C24" t="str">
+        <v>A007</v>
+      </c>
+      <c r="D24">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25">
+        <v>51</v>
+      </c>
+      <c r="B25" t="str">
+        <v>RnD</v>
+      </c>
+      <c r="C25" t="str">
+        <v>A106</v>
+      </c>
+      <c r="D25">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26">
+        <v>52</v>
+      </c>
+      <c r="B26" t="str">
+        <v>RnD</v>
+      </c>
+      <c r="C26" t="str">
+        <v>B105</v>
+      </c>
+      <c r="D26">
+        <v>42</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:D15"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:D26"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Invigilation page final step done.
</commit_message>
<xml_diff>
--- a/backend/media/invigilationFiles/Classroom.xlsx
+++ b/backend/media/invigilationFiles/Classroom.xlsx
@@ -418,352 +418,352 @@
     </row>
     <row r="2">
       <c r="A2">
-        <v>28</v>
+        <v>36</v>
       </c>
       <c r="B2" t="str">
         <v>Old Acad</v>
       </c>
       <c r="C2" t="str">
-        <v>C01</v>
+        <v>C24</v>
       </c>
       <c r="D2">
-        <v>106</v>
+        <v>18</v>
       </c>
     </row>
     <row r="3">
       <c r="A3">
-        <v>29</v>
+        <v>37</v>
       </c>
       <c r="B3" t="str">
-        <v>Old Acad</v>
+        <v>LHC</v>
       </c>
       <c r="C3" t="str">
-        <v>C02</v>
+        <v>C101</v>
       </c>
       <c r="D3">
-        <v>42</v>
+        <v>169</v>
       </c>
     </row>
     <row r="4">
       <c r="A4">
-        <v>30</v>
+        <v>38</v>
       </c>
       <c r="B4" t="str">
-        <v>Old Acad</v>
+        <v>LHC</v>
       </c>
       <c r="C4" t="str">
-        <v>C03</v>
+        <v>C102</v>
       </c>
       <c r="D4">
-        <v>18</v>
+        <v>281</v>
       </c>
     </row>
     <row r="5">
       <c r="A5">
-        <v>31</v>
+        <v>39</v>
       </c>
       <c r="B5" t="str">
-        <v>Old Acad</v>
+        <v>LHC</v>
       </c>
       <c r="C5" t="str">
-        <v>C11</v>
+        <v>C201</v>
       </c>
       <c r="D5">
-        <v>94</v>
+        <v>177</v>
       </c>
     </row>
     <row r="6">
       <c r="A6">
-        <v>32</v>
+        <v>40</v>
       </c>
       <c r="B6" t="str">
-        <v>Old Acad</v>
+        <v>LHC</v>
       </c>
       <c r="C6" t="str">
-        <v>C12</v>
+        <v>C208</v>
       </c>
       <c r="D6">
-        <v>39</v>
+        <v>20</v>
       </c>
     </row>
     <row r="7">
       <c r="A7">
-        <v>33</v>
+        <v>41</v>
       </c>
       <c r="B7" t="str">
-        <v>Old Acad</v>
+        <v>LHC</v>
       </c>
       <c r="C7" t="str">
-        <v>C13</v>
+        <v>C209</v>
       </c>
       <c r="D7">
-        <v>18</v>
+        <v>22</v>
       </c>
     </row>
     <row r="8">
       <c r="A8">
-        <v>34</v>
+        <v>42</v>
       </c>
       <c r="B8" t="str">
-        <v>Old Acad</v>
+        <v>LHC</v>
       </c>
       <c r="C8" t="str">
-        <v>C21</v>
+        <v>C210</v>
       </c>
       <c r="D8">
-        <v>80</v>
+        <v>25</v>
       </c>
     </row>
     <row r="9">
       <c r="A9">
-        <v>35</v>
+        <v>43</v>
       </c>
       <c r="B9" t="str">
         <v>Old Acad</v>
       </c>
       <c r="C9" t="str">
-        <v>C22</v>
+        <v>C211</v>
       </c>
       <c r="D9">
-        <v>18</v>
+        <v>24</v>
       </c>
     </row>
     <row r="10">
       <c r="A10">
-        <v>36</v>
+        <v>44</v>
       </c>
       <c r="B10" t="str">
-        <v>Old Acad</v>
+        <v>LHC</v>
       </c>
       <c r="C10" t="str">
-        <v>C24</v>
+        <v>C212</v>
       </c>
       <c r="D10">
-        <v>18</v>
+        <v>28</v>
       </c>
     </row>
     <row r="11">
       <c r="A11">
-        <v>37</v>
+        <v>45</v>
       </c>
       <c r="B11" t="str">
         <v>LHC</v>
       </c>
       <c r="C11" t="str">
-        <v>C101</v>
+        <v>C213</v>
       </c>
       <c r="D11">
-        <v>169</v>
+        <v>31</v>
       </c>
     </row>
     <row r="12">
       <c r="A12">
-        <v>38</v>
+        <v>46</v>
       </c>
       <c r="B12" t="str">
         <v>LHC</v>
       </c>
       <c r="C12" t="str">
-        <v>C102</v>
+        <v>C214</v>
       </c>
       <c r="D12">
-        <v>281</v>
+        <v>20</v>
       </c>
     </row>
     <row r="13">
       <c r="A13">
-        <v>39</v>
+        <v>47</v>
       </c>
       <c r="B13" t="str">
         <v>LHC</v>
       </c>
       <c r="C13" t="str">
-        <v>C201</v>
+        <v>C215</v>
       </c>
       <c r="D13">
-        <v>177</v>
+        <v>22</v>
       </c>
     </row>
     <row r="14">
       <c r="A14">
-        <v>40</v>
+        <v>48</v>
       </c>
       <c r="B14" t="str">
         <v>LHC</v>
       </c>
       <c r="C14" t="str">
-        <v>C208</v>
+        <v>C216</v>
       </c>
       <c r="D14">
-        <v>20</v>
+        <v>17</v>
       </c>
     </row>
     <row r="15">
       <c r="A15">
-        <v>41</v>
+        <v>49</v>
       </c>
       <c r="B15" t="str">
-        <v>LHC</v>
+        <v>RnD</v>
       </c>
       <c r="C15" t="str">
-        <v>C209</v>
+        <v>A006</v>
       </c>
       <c r="D15">
-        <v>22</v>
+        <v>58</v>
       </c>
     </row>
     <row r="16">
       <c r="A16">
-        <v>42</v>
+        <v>50</v>
       </c>
       <c r="B16" t="str">
-        <v>LHC</v>
+        <v>RnD</v>
       </c>
       <c r="C16" t="str">
-        <v>C210</v>
+        <v>A007</v>
       </c>
       <c r="D16">
-        <v>25</v>
+        <v>56</v>
       </c>
     </row>
     <row r="17">
       <c r="A17">
-        <v>43</v>
+        <v>51</v>
       </c>
       <c r="B17" t="str">
-        <v>Old Acad</v>
+        <v>RnD</v>
       </c>
       <c r="C17" t="str">
-        <v>C211</v>
+        <v>A106</v>
       </c>
       <c r="D17">
-        <v>24</v>
+        <v>48</v>
       </c>
     </row>
     <row r="18">
       <c r="A18">
-        <v>44</v>
+        <v>52</v>
       </c>
       <c r="B18" t="str">
-        <v>LHC</v>
+        <v>RnD</v>
       </c>
       <c r="C18" t="str">
-        <v>C212</v>
+        <v>B105</v>
       </c>
       <c r="D18">
-        <v>28</v>
+        <v>42</v>
       </c>
     </row>
     <row r="19">
       <c r="A19">
-        <v>45</v>
+        <v>53</v>
       </c>
       <c r="B19" t="str">
-        <v>LHC</v>
+        <v>Old Acad</v>
       </c>
       <c r="C19" t="str">
-        <v>C213</v>
+        <v>C01</v>
       </c>
       <c r="D19">
-        <v>31</v>
+        <v>100</v>
       </c>
     </row>
     <row r="20">
       <c r="A20">
-        <v>46</v>
+        <v>54</v>
       </c>
       <c r="B20" t="str">
-        <v>LHC</v>
+        <v>Old Acad</v>
       </c>
       <c r="C20" t="str">
-        <v>C214</v>
+        <v>C02</v>
       </c>
       <c r="D20">
-        <v>20</v>
+        <v>100</v>
       </c>
     </row>
     <row r="21">
       <c r="A21">
-        <v>47</v>
+        <v>55</v>
       </c>
       <c r="B21" t="str">
-        <v>LHC</v>
+        <v>Old Acad</v>
       </c>
       <c r="C21" t="str">
-        <v>C215</v>
+        <v>C03</v>
       </c>
       <c r="D21">
-        <v>22</v>
+        <v>100</v>
       </c>
     </row>
     <row r="22">
       <c r="A22">
-        <v>48</v>
+        <v>56</v>
       </c>
       <c r="B22" t="str">
-        <v>LHC</v>
+        <v>Old Acad</v>
       </c>
       <c r="C22" t="str">
-        <v>C216</v>
+        <v>C11</v>
       </c>
       <c r="D22">
-        <v>17</v>
+        <v>100</v>
       </c>
     </row>
     <row r="23">
       <c r="A23">
-        <v>49</v>
+        <v>57</v>
       </c>
       <c r="B23" t="str">
-        <v>RnD</v>
+        <v>Old Acad</v>
       </c>
       <c r="C23" t="str">
-        <v>A006</v>
+        <v>C04</v>
       </c>
       <c r="D23">
-        <v>58</v>
+        <v>100</v>
       </c>
     </row>
     <row r="24">
       <c r="A24">
-        <v>50</v>
+        <v>58</v>
       </c>
       <c r="B24" t="str">
         <v>RnD</v>
       </c>
       <c r="C24" t="str">
-        <v>A007</v>
+        <v>A105</v>
       </c>
       <c r="D24">
-        <v>56</v>
+        <v>100</v>
       </c>
     </row>
     <row r="25">
       <c r="A25">
-        <v>51</v>
+        <v>59</v>
       </c>
       <c r="B25" t="str">
-        <v>RnD</v>
+        <v>Old Acad</v>
       </c>
       <c r="C25" t="str">
-        <v>A106</v>
+        <v>C12</v>
       </c>
       <c r="D25">
-        <v>48</v>
+        <v>100</v>
       </c>
     </row>
     <row r="26">
       <c r="A26">
-        <v>52</v>
+        <v>60</v>
       </c>
       <c r="B26" t="str">
-        <v>RnD</v>
+        <v>Old Acad</v>
       </c>
       <c r="C26" t="str">
-        <v>B105</v>
+        <v>C21</v>
       </c>
       <c r="D26">
-        <v>42</v>
+        <v>100</v>
       </c>
     </row>
   </sheetData>

</xml_diff>